<commit_message>
created map with bar chart and arrow flow
</commit_message>
<xml_diff>
--- a/data/Table_sourcing_terremissions_by_c_2016-05-18.xlsx
+++ b/data/Table_sourcing_terremissions_by_c_2016-05-18.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sankey diagram" sheetId="1" r:id="rId1"/>
     <sheet name="Arrows on a map" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="33">
   <si>
     <t>US</t>
   </si>
@@ -73,15 +76,6 @@
     <t>Right bar</t>
   </si>
   <si>
-    <t xml:space="preserve">Row = Arrows from </t>
-  </si>
-  <si>
-    <t>Column = Arrows to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow mark = diagonal = Bar graph in each country = Within-territory emission reduction due to sourcing decision by the country </t>
-  </si>
-  <si>
     <t>Positive side</t>
   </si>
   <si>
@@ -126,6 +120,9 @@
   <si>
     <t>sum</t>
   </si>
+  <si>
+    <t>sourcing</t>
+  </si>
 </sst>
 </file>
 
@@ -134,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +142,22 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,22 +186,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -225,10 +246,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14375240594925634"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.82847112860892391"/>
-          <c:h val="0.89719889180519097"/>
+          <c:x val="0.143752405949256"/>
+          <c:y val="0.0514005540974045"/>
+          <c:w val="0.828471128608924"/>
+          <c:h val="0.897198891805191"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -277,7 +298,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>383904.27446958481</c:v>
+                  <c:v>383904.2744695848</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -325,7 +346,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>131810.68959695907</c:v>
+                  <c:v>131810.6895969591</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,7 +385,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>93495.634307597997</c:v>
+                  <c:v>93495.634307598</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -403,7 +424,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60268.433237795674</c:v>
+                  <c:v>60268.43323779567</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -442,7 +463,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>26750.517528484786</c:v>
+                  <c:v>26750.51752848479</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -481,7 +502,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19256.427398472457</c:v>
+                  <c:v>19256.42739847246</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,7 +541,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30550.986766950326</c:v>
+                  <c:v>30550.98676695033</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -568,7 +589,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>503.49520311442029</c:v>
+                  <c:v>503.4952031144203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,7 +637,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-285522.54640127893</c:v>
+                  <c:v>-285522.5464012789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -655,7 +676,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-51057.271448236635</c:v>
+                  <c:v>-51057.27144823664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,7 +715,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-79602.881994056035</c:v>
+                  <c:v>-79602.88199405603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,7 +754,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-54293.273646077236</c:v>
+                  <c:v>-54293.27364607724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -772,7 +793,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-4298.6315012670093</c:v>
+                  <c:v>-4298.63150126701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,7 +832,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-6656.1387256789676</c:v>
+                  <c:v>-6656.138725678967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -850,7 +871,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-29837.589741776432</c:v>
+                  <c:v>-29837.58974177643</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,7 +910,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-38468.703593902595</c:v>
+                  <c:v>-38468.7035939026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,11 +926,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="77853184"/>
-        <c:axId val="90890816"/>
+        <c:axId val="2125281464"/>
+        <c:axId val="2126066104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77853184"/>
+        <c:axId val="2125281464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -918,7 +939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90890816"/>
+        <c:crossAx val="2126066104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -926,7 +947,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90890816"/>
+        <c:axId val="2126066104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77853184"/>
+        <c:crossAx val="2125281464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -979,10 +1000,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14375240594925634"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.82847112860892391"/>
-          <c:h val="0.89719889180519097"/>
+          <c:x val="0.143752405949256"/>
+          <c:y val="0.0514005540974045"/>
+          <c:w val="0.828471128608924"/>
+          <c:h val="0.897198891805191"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1022,7 +1043,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>12525.755828584171</c:v>
+                  <c:v>12525.75582858417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,7 +1082,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7338.4997974467478</c:v>
+                  <c:v>7338.499797446748</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,7 +1121,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>36881.065452684888</c:v>
+                  <c:v>36881.06545268489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1139,7 +1160,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1082.9391578161587</c:v>
+                  <c:v>1082.939157816159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1178,7 +1199,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9739.5480886802216</c:v>
+                  <c:v>9739.548088680221</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1217,7 +1238,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>42728.537431593126</c:v>
+                  <c:v>42728.53743159313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1256,7 +1277,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4023.0236422938206</c:v>
+                  <c:v>4023.023642293821</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,7 +1325,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>681462.70414039551</c:v>
+                  <c:v>681462.7041403955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,7 +1373,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-306411.93731530494</c:v>
+                  <c:v>-306411.937315305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,7 +1412,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-53129.138799863358</c:v>
+                  <c:v>-53129.13879986336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1430,7 +1451,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-79602.881994056035</c:v>
+                  <c:v>-79602.88199405603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1469,7 +1490,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-67389.797135569257</c:v>
+                  <c:v>-67389.79713556926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,7 +1529,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-4344.7224842150263</c:v>
+                  <c:v>-4344.722484215026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1547,7 +1568,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-14272.529055169629</c:v>
+                  <c:v>-14272.52905516963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1625,7 +1646,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-38468.703593902595</c:v>
+                  <c:v>-38468.7035939026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1641,11 +1662,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="164398080"/>
-        <c:axId val="90897728"/>
+        <c:axId val="2126120152"/>
+        <c:axId val="2126123096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164398080"/>
+        <c:axId val="2126120152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1654,15 +1675,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90897728"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="2126123096"/>
+        <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90897728"/>
+        <c:axId val="2126123096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164398080"/>
+        <c:crossAx val="2126120152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1805,6 +1826,90 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2260600" y="2298700"/>
+          <a:ext cx="4914900" cy="2552700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Row = Arrows from </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Column = Arrows to</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Yellow mark = diagonal = Bar graph in each country = Within-territory emission reduction due to sourcing decision by the country </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1848,7 +1953,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1883,7 +1988,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2060,7 +2165,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2070,17 +2175,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="9" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2133,10 +2238,10 @@
         <v>7</v>
       </c>
       <c r="V1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2209,7 +2314,7 @@
         <v>-285522.54640127893</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2249,7 +2354,7 @@
         <v>-51057.271448236635</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2289,7 +2394,7 @@
         <v>-79602.881994056035</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2322,7 +2427,7 @@
         <v>5975.1595917184386</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U5" t="s">
         <v>3</v>
@@ -2332,7 +2437,7 @@
         <v>-54293.273646077236</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2404,7 +2509,7 @@
         <v>-4298.6315012670093</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2444,7 +2549,7 @@
         <v>-6656.1387256789676</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2477,7 +2582,7 @@
         <v>713.39702517389378</v>
       </c>
       <c r="L8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="U8" t="s">
         <v>6</v>
@@ -2487,7 +2592,7 @@
         <v>-29837.589741776432</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2559,7 +2664,7 @@
         <v>-38468.703593902595</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2600,7 +2705,7 @@
         <v>196803.42145668564</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -2629,22 +2734,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -2658,9 +2763,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
+    <row r="18" spans="1:7">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -2669,8 +2774,8 @@
         <f>J2-V2</f>
         <v>383904.27446958481</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>25</v>
+      <c r="D18" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="F18" t="s">
         <v>0</v>
@@ -2680,8 +2785,8 @@
         <v>12525.755828584171</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -2689,8 +2794,8 @@
         <f t="shared" ref="C19:C25" si="6">J3-V3</f>
         <v>131810.68959695907</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>26</v>
+      <c r="D19" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F19" t="s">
         <v>1</v>
@@ -2700,8 +2805,8 @@
         <v>7338.4997974467478</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:7">
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -2709,8 +2814,8 @@
         <f t="shared" si="6"/>
         <v>93495.634307597997</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>27</v>
+      <c r="D20" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="F20" t="s">
         <v>2</v>
@@ -2720,8 +2825,8 @@
         <v>36881.065452684888</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -2729,8 +2834,8 @@
         <f t="shared" si="6"/>
         <v>60268.433237795674</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>28</v>
+      <c r="D21" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F21" t="s">
         <v>3</v>
@@ -2740,8 +2845,8 @@
         <v>1082.9391578161587</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:7">
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -2749,8 +2854,8 @@
         <f t="shared" si="6"/>
         <v>26750.517528484786</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>29</v>
+      <c r="D22" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>
@@ -2760,8 +2865,8 @@
         <v>9739.5480886802216</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>5</v>
       </c>
@@ -2769,8 +2874,8 @@
         <f t="shared" si="6"/>
         <v>19256.427398472457</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>30</v>
+      <c r="D23" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="F23" t="s">
         <v>5</v>
@@ -2780,8 +2885,8 @@
         <v>42728.537431593126</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5"/>
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -2789,8 +2894,8 @@
         <f t="shared" si="6"/>
         <v>30550.986766950326</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>31</v>
+      <c r="D24" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
@@ -2800,8 +2905,8 @@
         <v>4023.0236422938206</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:7">
+      <c r="A25" s="5"/>
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -2809,8 +2914,8 @@
         <f t="shared" si="6"/>
         <v>503.49520311442029</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>32</v>
+      <c r="D25" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
@@ -2820,9 +2925,9 @@
         <v>681462.70414039551</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>22</v>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -2831,8 +2936,8 @@
         <f>V2</f>
         <v>-285522.54640127893</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>33</v>
+      <c r="D26" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F26" t="s">
         <v>0</v>
@@ -2842,8 +2947,8 @@
         <v>-306411.93731530494</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:7">
+      <c r="A27" s="5"/>
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -2851,8 +2956,8 @@
         <f t="shared" ref="C27:C33" si="8">V3</f>
         <v>-51057.271448236635</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>33</v>
+      <c r="D27" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F27" t="s">
         <v>1</v>
@@ -2862,8 +2967,8 @@
         <v>-53129.138799863358</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5"/>
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -2871,8 +2976,8 @@
         <f t="shared" si="8"/>
         <v>-79602.881994056035</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>33</v>
+      <c r="D28" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F28" t="s">
         <v>2</v>
@@ -2882,8 +2987,8 @@
         <v>-79602.881994056035</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5"/>
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -2891,8 +2996,8 @@
         <f t="shared" si="8"/>
         <v>-54293.273646077236</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>33</v>
+      <c r="D29" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
@@ -2902,8 +3007,8 @@
         <v>-67389.797135569257</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5"/>
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -2911,8 +3016,8 @@
         <f t="shared" si="8"/>
         <v>-4298.6315012670093</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>33</v>
+      <c r="D30" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
@@ -2922,8 +3027,8 @@
         <v>-4344.7224842150263</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+    <row r="31" spans="1:7">
+      <c r="A31" s="5"/>
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -2931,8 +3036,8 @@
         <f t="shared" si="8"/>
         <v>-6656.1387256789676</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>33</v>
+      <c r="D31" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F31" t="s">
         <v>5</v>
@@ -2942,8 +3047,8 @@
         <v>-14272.529055169629</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5"/>
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -2951,8 +3056,8 @@
         <f t="shared" si="8"/>
         <v>-29837.589741776432</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>33</v>
+      <c r="D32" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -2962,8 +3067,8 @@
         <v>-35358.94170472808</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5"/>
       <c r="B33" t="s">
         <v>7</v>
       </c>
@@ -2971,8 +3076,8 @@
         <f t="shared" si="8"/>
         <v>-38468.703593902595</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>33</v>
+      <c r="D33" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F33" t="s">
         <v>7</v>
@@ -2982,9 +3087,9 @@
         <v>-38468.703593902595</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1">
         <f>SUM(C18:C33)</f>
@@ -2995,7 +3100,7 @@
         <v>196803.4214566857</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="B38" t="s">
         <v>15</v>
       </c>
@@ -3010,26 +3115,31 @@
     <mergeCell ref="A26:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="9" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3058,7 +3168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3115,7 +3225,7 @@
         <v>2843.811712126158</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3172,7 +3282,7 @@
         <v>-1741.1560952149136</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3229,7 +3339,7 @@
         <v>1175.2829797359061</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3286,7 +3396,7 @@
         <v>-2435.3076174775938</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3343,7 +3453,7 @@
         <v>327.40608804491347</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3400,7 +3510,7 @@
         <v>1431.2897969647058</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3457,7 +3567,7 @@
         <v>-1097.8316610647566</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3514,7 +3624,7 @@
         <v>-38468.703593902595</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3555,9 +3665,7 @@
         <v>196803.42145668564</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -3586,7 +3694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -3627,7 +3735,7 @@
         <v>392267.90955502668</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -3668,7 +3776,7 @@
         <v>126544.05715113904</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -3709,7 +3817,7 @@
         <v>56614.568854913101</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -3750,7 +3858,7 @@
         <v>72282.017569471529</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3791,7 +3899,7 @@
         <v>17057.060422752584</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3832,7 +3940,7 @@
         <v>-15855.719703629999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -3873,7 +3981,7 @@
         <v>32049.315087608149</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -3914,7 +4022,7 @@
         <v>-680959.20893728104</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -3955,11 +4063,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="C23" s="2"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -3988,7 +4099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -4029,7 +4140,7 @@
         <v>109513.76220490452</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -4070,7 +4181,7 @@
         <v>89997.138219070388</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -4111,7 +4222,7 @@
         <v>-1910.0537329154467</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -4152,7 +4263,7 @@
         <v>18206.645177025759</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -4193,7 +4304,7 @@
         <v>29579.224372938275</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -4234,7 +4345,7 @@
         <v>29895.417946630063</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -4275,7 +4386,7 @@
         <v>10672.234625031448</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -4316,7 +4427,7 @@
         <v>-38468.703593902595</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -4357,23 +4468,14 @@
         <v>247485.66521878238</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>